<commit_message>
Testes concluidos + README
</commit_message>
<xml_diff>
--- a/results/comparative_results.xlsx
+++ b/results/comparative_results.xlsx
@@ -8,6 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="N=500" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="N=1000" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="N=5000" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="N=30000" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="N=80000" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="N=100000" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="N=150000" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="N=200000" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,7 +448,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.2889 ms</t>
+          <t>0.2921 ms</t>
         </is>
       </c>
     </row>
@@ -453,7 +460,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5.0673 ms</t>
+          <t>0.2277 ms</t>
         </is>
       </c>
     </row>
@@ -465,7 +472,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.5354 ms</t>
+          <t>0.5152 ms</t>
         </is>
       </c>
     </row>
@@ -477,7 +484,560 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.4494 ms</t>
+          <t>0.5322 ms</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Algoritmo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tempo Médio (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Quicksort (Hoare)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0.5890 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Quicksort (Lomuto)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.5198 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Heapsort</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.1673 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mergesort</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.1726 ms</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Algoritmo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tempo Médio (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Quicksort (Hoare)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3.5785 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Quicksort (Lomuto)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3.4315 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Heapsort</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>7.4780 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mergesort</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>7.4222 ms</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Algoritmo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tempo Médio (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Quicksort (Hoare)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>24.8624 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Quicksort (Lomuto)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>24.3914 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Heapsort</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>54.6847 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mergesort</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>51.5753 ms</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Algoritmo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tempo Médio (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Quicksort (Hoare)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>73.5334 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Quicksort (Lomuto)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>69.7008 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Heapsort</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>167.8666 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mergesort</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>149.9654 ms</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Algoritmo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tempo Médio (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Quicksort (Hoare)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>91.9338 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Quicksort (Lomuto)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>86.2856 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Heapsort</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>211.1490 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mergesort</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>190.1577 ms</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Algoritmo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tempo Médio (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Quicksort (Hoare)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>140.8679 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Quicksort (Lomuto)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>143.9973 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Heapsort</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>321.5176 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mergesort</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>298.4678 ms</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Algoritmo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Tempo Médio (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Quicksort (Hoare)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.1683 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Quicksort (Lomuto)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>187.8450 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Heapsort</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>444.4166 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mergesort</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>400.8666 ms</t>
         </is>
       </c>
     </row>

</xml_diff>